<commit_message>
prepare presentation for wit
</commit_message>
<xml_diff>
--- a/Score_analysis/Firstouts.xlsx
+++ b/Score_analysis/Firstouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janiswaser/Desktop/Conversion/Score_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE477ABF-C8CF-E847-A8F8-0B14AB418E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6EC7D7-708C-2749-8DA9-3198A6BA2021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="-20660" windowWidth="20580" windowHeight="17440" xr2:uid="{B54BFC66-9CB4-CF48-B46C-4A8CA942E9A1}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{B54BFC66-9CB4-CF48-B46C-4A8CA942E9A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,10 +83,10 @@
     <t>Mean, Var</t>
   </si>
   <si>
-    <t>0, 0.21</t>
-  </si>
-  <si>
-    <t>0, 0.086</t>
+    <t>1.1, 0.096</t>
+  </si>
+  <si>
+    <t>0, 0.23</t>
   </si>
 </sst>
 </file>
@@ -94,8 +94,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.000000%"/>
-    <numFmt numFmtId="181" formatCode="0.00000000%"/>
+    <numFmt numFmtId="164" formatCode="0.000000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000000%"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -191,9 +191,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355B59E6-ADE6-0A4F-8822-3E57EF3C405F}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,13 +546,13 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q1" t="s">
         <v>14</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -613,21 +613,21 @@
         <v>358117.5</v>
       </c>
       <c r="N3" s="12">
-        <v>2.0444199999999999E-8</v>
+        <v>8.9321010000000006E-8</v>
       </c>
       <c r="O3" s="11">
         <f t="shared" ref="O3:O5" si="0">N3</f>
-        <v>2.0444199999999999E-8</v>
+        <v>8.9321010000000006E-8</v>
       </c>
       <c r="P3">
         <v>2.57</v>
       </c>
       <c r="Q3" s="10">
-        <v>5.8983719999999997E-8</v>
+        <v>3.3427959999999999E-6</v>
       </c>
       <c r="R3" s="11">
         <f>Q3</f>
-        <v>5.8983719999999997E-8</v>
+        <v>3.3427959999999999E-6</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -668,21 +668,21 @@
         <v>765307</v>
       </c>
       <c r="N4" s="12">
-        <v>2.9264920000000003E-7</v>
+        <v>1.011073E-6</v>
       </c>
       <c r="O4" s="11">
         <f t="shared" si="0"/>
-        <v>2.9264920000000003E-7</v>
+        <v>1.011073E-6</v>
       </c>
       <c r="P4">
         <v>2.35</v>
       </c>
       <c r="Q4" s="10">
-        <v>2.9877339999999999E-6</v>
+        <v>7.7226799999999997E-5</v>
       </c>
       <c r="R4" s="11">
-        <f t="shared" ref="R4:R5" si="1">Q4</f>
-        <v>2.9877339999999999E-6</v>
+        <f t="shared" ref="R4" si="1">Q4</f>
+        <v>7.7226799999999997E-5</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -723,21 +723,21 @@
         <v>555449</v>
       </c>
       <c r="N5" s="12">
-        <v>9.431039E-6</v>
+        <v>2.4035519999999999E-5</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" si="0"/>
-        <v>9.431039E-6</v>
+        <v>2.4035519999999999E-5</v>
       </c>
       <c r="P5">
         <v>2.0299999999999998</v>
       </c>
       <c r="Q5" s="10">
-        <v>3.4297640000000002E-4</v>
+        <v>3.272409E-3</v>
       </c>
       <c r="R5" s="11">
         <f>Q5</f>
-        <v>3.4297640000000002E-4</v>
+        <v>3.272409E-3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>